<commit_message>
[FIX] for test data
</commit_message>
<xml_diff>
--- a/admin/features_files/historic/Features_Base.xlsx
+++ b/admin/features_files/historic/Features_Base.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
   <si>
     <t>Nom des phases de description (description de soi, d'autrui, …)</t>
   </si>
@@ -69,12 +69,6 @@
     <t>physique-2</t>
   </si>
   <si>
-    <t>attitude</t>
-  </si>
-  <si>
-    <t>autres</t>
-  </si>
-  <si>
     <t>Nom de la feature (Texte affiché sur la carte lors de la phase de classement)</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>Signes particuliers (grains de beauté, taches de rousseur, bronzage, tatouages, piercings...)</t>
   </si>
   <si>
-    <t>Sous-vêtements</t>
-  </si>
-  <si>
     <t>Couleur des yeux</t>
   </si>
   <si>
@@ -153,61 +144,7 @@
     <t>Style d'habillement du soir</t>
   </si>
   <si>
-    <t>Style de vêtement en lien avec la personnalité (bab, cutester, BCBG, bohème, chic, classique, décontracté, electro, excentrique, fluo)</t>
-  </si>
-  <si>
-    <t>Consommation d'alcool et fréquence</t>
-  </si>
-  <si>
-    <t>Consommation du tabac et fréquence</t>
-  </si>
-  <si>
-    <t>Régime alimentaire, habitudes, plats préférés, importance accordée aux repas</t>
-  </si>
-  <si>
-    <t>S'exposer en photos</t>
-  </si>
-  <si>
-    <t>S'exposer en vidéos</t>
-  </si>
-  <si>
-    <t>Orientation sexuelle (hétéro, homo, bi, trans)</t>
-  </si>
-  <si>
-    <t>Fétichisme avec des vêtements (cuir, équipement de sports, skateur.se, caoutchouc, sous-vêtements, peaux et punks, bottes, lycra, uniforme, robe de soirée, raver, bas et bas, jeans, lingerie, travailleur)</t>
-  </si>
-  <si>
-    <t>Genre (agender, androgyne, asexué, bigender, cisgender, cisgender...)</t>
-  </si>
-  <si>
-    <t>Talents culinaires</t>
-  </si>
-  <si>
-    <t>Statut VIH</t>
-  </si>
-  <si>
     <t>Lunettes ou lentilles de contact</t>
-  </si>
-  <si>
-    <t>Maladies sexuellement transmissibles (Verrues génitales, Herpès type I, Herpès type II…)</t>
-  </si>
-  <si>
-    <t>S'exposer en Webcam</t>
-  </si>
-  <si>
-    <t>Mode et marques</t>
-  </si>
-  <si>
-    <t>Sports préférés, sports pratiqués, fréquence de la pratique</t>
-  </si>
-  <si>
-    <t>Satisfaction de l'apparence physique</t>
-  </si>
-  <si>
-    <t>L'âge dans la tête</t>
-  </si>
-  <si>
-    <t>Dates de rappels de pistage</t>
   </si>
   <si>
     <t>Premièrement, vous allez classer les caractéristiques qui vous définissent le plus.
@@ -222,9 +159,6 @@
   </si>
   <si>
     <t>Quel est le sexe par lequel vous êtes attiré.e ?</t>
-  </si>
-  <si>
-    <t>Quelles sont les caractéristiques auxquelles vous accordez de l'importance lors d'une rencontre ?</t>
   </si>
   <si>
     <t>Quelles sont les caractéristiques corporelles auxquelles vous accordez de l'importance lors d'une rencontre ?</t>
@@ -603,7 +537,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -612,7 +546,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -620,7 +554,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
@@ -629,7 +563,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -642,10 +576,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -672,7 +606,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -686,55 +620,33 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 A5:B5 A4:B4 D4:E4 D5:E5 A3:B3 D3:E3 A2:B2 D2:E2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E1 D4:E4 D5:E5 A3:B3 D3:E3 A2:B2 D2:E2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -745,7 +657,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -759,7 +671,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -773,7 +685,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -787,7 +699,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -801,7 +713,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -815,7 +727,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -829,7 +741,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -843,7 +755,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -857,7 +769,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -871,7 +783,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -885,7 +797,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -899,7 +811,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
@@ -913,63 +825,63 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -983,7 +895,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
@@ -997,7 +909,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -1011,7 +923,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
@@ -1025,7 +937,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
         <v>16</v>
@@ -1039,7 +951,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
         <v>16</v>
@@ -1048,286 +960,6 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1335,7 +967,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D2 A4:D31 B3:D3 A33:D43 B32:D32" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D2 A4:D23 B3:D3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>